<commit_message>
link to coverage in Zifencei isa vplan
Signed-off-by: Robin Pedersen <Robin.Pedersen@silabs.com>
</commit_message>
<xml_diff>
--- a/docs/VerifPlans/ISA/RV32/Simulation/RV32Zifencei_Extension_Instruction.xlsx
+++ b/docs/VerifPlans/ISA/RV32/Simulation/RV32Zifencei_Extension_Instruction.xlsx
@@ -1,32 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ropeders\Documents\vplan_covlinks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E59D8D0-E3E8-4B36-A720-1F0902A63004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CCFF9A-02BD-48B9-9BA3-EC7BB8CCFB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="915" windowWidth="26475" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RV32Z" sheetId="1" r:id="rId1"/>
     <sheet name="DONOTDELETE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -128,14 +123,31 @@
   <si>
     <t>Fence.I instruction executed
 Implementation is core-specific</t>
+  </si>
+  <si>
+    <t>isacov_agent.cov_model.rv32zifencei_fence_i_cg</t>
+  </si>
+  <si>
+    <t>Missing Coverage</t>
+  </si>
+  <si>
+    <t>This only tracks that the instruction was executed. Refer to the vplans for the core under test for specific instruction test and coverage.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -148,27 +160,12 @@
       <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
     </font>
   </fonts>
   <fills count="3">
@@ -197,52 +194,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,48 +598,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="35.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="59.42578125" style="3" customWidth="1"/>
-    <col min="10" max="1023" width="17" style="3"/>
-    <col min="1024" max="1024" width="9.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="35.44140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="59.44140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="32.44140625" style="4" customWidth="1"/>
+    <col min="11" max="1023" width="17" style="4"/>
+    <col min="1024" max="1024" width="9.109375" style="4" customWidth="1"/>
+    <col min="1025" max="16384" width="17" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" ht="30">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="6" t="s">
@@ -676,77 +650,52 @@
       <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" ht="28.5">
-      <c r="A2" s="14" t="s">
+      <c r="J1" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="89.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" s="10" customFormat="1">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" s="10" customFormat="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="1:9" s="12" customFormat="1">
-      <c r="A5" s="13" t="s">
+      <c r="I2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -782,27 +731,27 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="15" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -813,7 +762,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -824,7 +773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -835,7 +784,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -846,7 +795,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -857,7 +806,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -865,7 +814,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -873,7 +822,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>

</xml_diff>